<commit_message>
Updated autoemailsender to add the current time in the excel spreadsheet for when it was first sent, and the second time.
</commit_message>
<xml_diff>
--- a/email_list.xlsx
+++ b/email_list.xlsx
@@ -1,40 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Boo\Desktop\git-projects\objective-python-course\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41345E16-0093-4387-B5DB-2DDC1135737C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="9260" xr2:uid="{71701719-1F72-410A-8FE3-DA207163F9E4}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9255" windowWidth="20475" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>Asset</t>
   </si>
   <si>
@@ -50,74 +37,81 @@
     <t>Model</t>
   </si>
   <si>
+    <t>First Email</t>
+  </si>
+  <si>
+    <t>Second Email</t>
+  </si>
+  <si>
     <t>Jake Burgess</t>
   </si>
   <si>
+    <t>jake.p.burgess@gmail.com</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>X1 Carbon</t>
+  </si>
+  <si>
+    <t>James Brown</t>
+  </si>
+  <si>
     <t>Desktop</t>
   </si>
   <si>
-    <t>Lenovo</t>
-  </si>
-  <si>
-    <t>X1 Carbon</t>
-  </si>
-  <si>
-    <t>James Brown</t>
-  </si>
-  <si>
-    <t>Laptop</t>
-  </si>
-  <si>
     <t>M910 Tiny</t>
   </si>
   <si>
+    <t>Mark Smith</t>
+  </si>
+  <si>
     <t>Dell</t>
   </si>
   <si>
     <t>Dell Optiplex 9020</t>
-  </si>
-  <si>
-    <t>Mark Smith</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>jake.p.burgess@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="yyyy\-mm\-dd" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
+  </numFmts>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -133,28 +127,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -454,120 +441,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126C103C-0211-42C1-83F8-332094013A5F}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B2:B4"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="18.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="24.140625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="14.42578125"/>
+    <col customWidth="1" max="5" min="5" width="12.140625"/>
+    <col customWidth="1" max="7" min="7" width="16.42578125"/>
+    <col customWidth="1" max="8" min="8" width="23.5703125"/>
+    <col customWidth="1" max="9" min="9" width="13.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
         <v>12000</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>1607</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>43562</v>
+      </c>
+      <c r="I2" s="3" t="n">
+        <v>43562</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="n">
+        <v>12005</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1709</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>43562</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>43562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="C3">
-        <v>12005</v>
-      </c>
-      <c r="D3">
-        <v>1709</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
         <v>13453</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>1703</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>43562</v>
+      </c>
+      <c r="I4" s="4" t="n">
+        <v>43562</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{843372C9-94B9-4F4F-9B69-0EB0580C67FC}"/>
-    <hyperlink ref="B2:B3" r:id="rId2" display="jake.p.burgess@gmail.com" xr:uid="{20374EB0-50F5-4F81-B2CC-D6A0267A49EE}"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B3" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B4" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>